<commit_message>
Testing, Classification Results and Corpus
</commit_message>
<xml_diff>
--- a/Documentation/Design Documents/Website Testing.xlsx
+++ b/Documentation/Design Documents/Website Testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\Documents\Coursework- Assignments\CO600 Project\project\co600\Documentation\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E41A48-E60C-4DEE-8CAC-08AA2FC4AE9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C40C4E5-F8AA-43DD-8F77-FB47336D9CAB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{53579F0D-9274-4238-9ABC-094FC6845497}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>Webpage split up into 3 sections and can be easily accessed through header menu</t>
   </si>
   <si>
-    <t>Tested in Chrome, Internet Explorer and Safari</t>
+    <t>Tested in Chrome, Internet Explorer, Safari and Firefox</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D2F33D-B39C-42D8-BD21-E8BC63A01C92}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>